<commit_message>
Prem | cuttack data with oriya
</commit_message>
<xml_diff>
--- a/routedata/Cuttack_PIS.xlsx
+++ b/routedata/Cuttack_PIS.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tanwisha.Mahapatra\Downloads\PIS\New folder\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FB4014-ECC5-4B4E-A2C5-318A390C2349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lot-1_36 Buses" sheetId="1" state="hidden" r:id="rId1"/>
@@ -19,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Cuttack!$A$3:$R$50</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="437">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -998,16 +992,393 @@
   </si>
   <si>
     <t>Via- Chahapada (Chhatratota)-Mahanga-Osanga-Pallisahi-Bhaunria-Umara-Gotara (Asulpur)-</t>
+  </si>
+  <si>
+    <t>ବାଙ୍କି-ପୁଇଞ୍ଚା |</t>
+  </si>
+  <si>
+    <t>ବାଙ୍କି-ବନସାପୁଟ |</t>
+  </si>
+  <si>
+    <t>ବାରଙ୍ଗା-ସିସୋ |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ବାରଙ୍ଗା-ତାଲାଗର |</t>
+  </si>
+  <si>
+    <t>କଣ୍ଟାପଡା-ନହଲପୁର |</t>
+  </si>
+  <si>
+    <t>କଣ୍ଟାପଡା-ପୋଷ୍ଟାଲା |</t>
+  </si>
+  <si>
+    <t>କଣ୍ଟାପଡା-ଦିମିନି |</t>
+  </si>
+  <si>
+    <t>ନରସିଂହପୁର-ଗୋଡିବନ୍ଧ</t>
+  </si>
+  <si>
+    <t>ନରସିଂହପୁର-ଚକାମୁଣ୍ଡା |</t>
+  </si>
+  <si>
+    <t>ନିଆଲି-ଏରଞ୍ଚା |</t>
+  </si>
+  <si>
+    <t>ନିଆଲି-ନିଭାରନ୍ |</t>
+  </si>
+  <si>
+    <t>ପଞ୍ଚାଗାନ୍ (ଟିଗିରିଆ) -ସାମପୁର |</t>
+  </si>
+  <si>
+    <t>କଣ୍ଟାପଡା-କଟକ |</t>
+  </si>
+  <si>
+    <t>ନରସିଂହପୁର-କଟକ |</t>
+  </si>
+  <si>
+    <t>ସାଲେପୁର-କଟକ |</t>
+  </si>
+  <si>
+    <t>ଟିଗିରିଆ-କଟକ |</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବନାବିଧ୍ୟାଧରପୁର-ଗାତିରାଉଟପାଟାନା-ବିରିବତୀ-ନିମାଇସାପୁର-କନ୍ଦରପୁର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ନୁଆପଡା ଚାକା-ଘାଟାକୁଲା ଚାକା-ink ିଙ୍କିରିଆ ଚାକା-ଶ୍ରୀରାମ-ବେଣ୍ଟାକର ଚାକା-ସିସୁଆ-ତାଇଲାପଡା-ରାଉତାପୁର-ଡେଲୁଲି-ତାଇକାନା-କାଲାପଡା-ଧିଆ-ବାରାଲ-କୁଲାସୁରିଚୁଆନ୍-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଗୋପାଳପୁର-ଶ୍ରୀକୋରୁଆନ୍-ଉରାଲୀ-ଜରିପଡା-ଖଣ୍ଡେଟା ଜିପି-ନାଗାବଲି-ସାଙ୍କତ୍ରାଶ-ନାଗାବଲି-ଆମାନା ଜିପି-ଅମାନପାରା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସୁନାପାଲ-ଭଟ୍ଟାରିକା ଛକା-ବାଦକମ୍ବିଲୋ-ଟିନିଗରିଆ-ଟେଲିକମ୍ବିଲୋ-ମାଣ୍ଡିଆପାଲ୍ଲୀ-ଧେଣ୍ଡାଖମ୍ବା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସୁନାପାଲା ଛକା-କଦମ୍ପଲ-ଗୋପପୁର-କୃଷ୍ଣଚନ୍ଦ୍ରପୁର-ଦାମଙ୍ଗାଡିଆ-ରତାପତ-ଦଶରଥୀପୁର</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ଭାୟା- ଅନୁରୀ-ଗୋଲାଗାଣ୍ଡା-ବ ide ଦେଶ୍ୱର-ବାଲାଭଦ୍ରପୁର-ଜଗନ୍ଥପୁର |_x000D_
+କେନ୍ଦୁ up ରୀ- </t>
+  </si>
+  <si>
+    <t>ଭାୟା- ମହିଦାରବାରା-ନାଗରୀ-ଡାଲବାଦ୍-କୁରଙ୍ଗ-ପ୍ରଦାନ-ଗଙ୍ଗେଶ୍ୱର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଚାହାପଡା (ଛତ୍ରୋଟା) -ମହଙ୍ଗା-ବାରାହିପୁର-ଓସଙ୍ଗା-ଗୋକାନ୍ (ଇରାକାନା) -ପୋଡାମରାଇ-ନାହଙ୍ଗା (ଗୋଦାଗୋପା ବଜାର) -ଭଦ୍ରାଶ୍ୱର-ଗୋପାଳପୁର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଚାହାପଡା (ଛତ୍ରୋଟା) -ମାଙ୍ଗା-ଓସଙ୍ଗା-ପଲ୍ଲିସାହି-ଭ un ନରିଆ-ଉମାରା-ଗୋଟାରା (ଅସୁଲପୁର) -</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ପାଇକାପଡାପାଟାନା-ଆଲାରା-ବାନ୍ଧହୁଦା-ଆଡେଇସୁଣ୍ଡି ସାଗର-ବୋକଡା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବାଲିସାହି-ସିସୁଆ-ସ uri ରୀ ଏବଂ ନନ୍ଦୋଲ-ମହାନ୍-କତାରପା-ଓଡିସିଂହ-ମାଲାସାନ-ନରଡା-ରମେଶ୍ୱର-ଗୋପୀନାଥପୁର-ସତ୍ୟଭାମପୁର-ବାହୁଗ୍ରାମ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ମହଲଦୀପା-ସମପଡା-ଖାନ୍ଦାହାଟା-ବାଦାନାପୁଟ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ପାସ୍-ବାଲିପୁଟ-ପଙ୍କଲ-ଭେଜିଆ-ଭୋଗଡା-ନୁଆପାଟାନା ଦ୍ୱାରା ନିଜିଗଡ଼-ବିନ୍ଦାନିମା-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">କଟକ ସଦର-ଆୟତପୁର </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ଆଠଗଡ-ଅନନ୍ତପୁର </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ଆଠଗଡ-ଗୋବୋରା </t>
+  </si>
+  <si>
+    <t>ବଡମ୍ବା -ଜୋଡୁମୁ |</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସାନାବରସିଂ-ରାଗଦୀପଡା-ଡିନାରୀ-ରାଗଦୀପଡା-ସାନାବରସିଂ-ବଡମ୍ବା-ସୁନାପାଲ-ଇଚାପୁର-ମଙ୍ଗରାଜପୁର-ସାଙ୍କାମୋରୀ-ଗୋପାମାଥୁରା-ଗୋପୀନାଥପୁର-ମୁଗାଗିରି-ବଙ୍ଗରିସିଂହା-ଯୋଡୁମୁ-ବଙ୍ଗରିସିଂହ-ମୁଗାଗାହିର-ଗୋପନାଥପୁର ଅଲ-ବଡମ୍ବା-</t>
+  </si>
+  <si>
+    <t>ବଡମ୍ବା-ଚାନଚୁନିଆ |</t>
+  </si>
+  <si>
+    <t>ବଡମ୍ବା-ମାଲାଟି |</t>
+  </si>
+  <si>
+    <t>ବଡମ୍ବା-ବିଶ୍ୱନାଥପୁର |</t>
+  </si>
+  <si>
+    <t>ବଡମ୍ବା-କଟକ |</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ବାରଙ୍ଗା-ନଛିପୁର </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>|</t>
+    </r>
+  </si>
+  <si>
+    <t>ଦାମପାରା-ପାଟପୁର  |</t>
+  </si>
+  <si>
+    <t>ଦାମପାରା-ତୁଳସୀପୁର  |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">କଟକ ସଦର- ଅର୍ଥଙ୍ଗ 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">କଟକ ସଦର- ଚାନ୍ଦୁଳି </t>
+  </si>
+  <si>
+    <t xml:space="preserve">କଟକ ସଦର-ବାମ୍ପକୁଦା </t>
+  </si>
+  <si>
+    <t>ଆଠଗଡ-ବଡ଼ଭୂଇଁଦେଶ  |</t>
+  </si>
+  <si>
+    <t>ବାଙ୍କି-କଳାପଥର  |</t>
+  </si>
+  <si>
+    <t>ବାଙ୍କି-କାଣ୍ଟପାନହରା |</t>
+  </si>
+  <si>
+    <t>କୁଆଁପାଳ  - କୁରୁଜଙ୍ଗ |</t>
+  </si>
+  <si>
+    <t>କୁଆଁପାଳ  - ହଳଦିଆ  |</t>
+  </si>
+  <si>
+    <t>କୁଆଁପାଳ  - ଗୋଟାରା (ଅସୁଲପୁର)</t>
+  </si>
+  <si>
+    <t>ନରସିଂହପୁର-ଦେବଭୂଇଁ  |</t>
+  </si>
+  <si>
+    <t>ନିଆଲି-ତିହୁଡି |</t>
+  </si>
+  <si>
+    <t>ନିଆଲି-ନୂଆଗାଁ  |</t>
+  </si>
+  <si>
+    <t>ନିଶ୍ଚିନ୍ତକୋଇଲି  - ଉତରକୁଳ  |</t>
+  </si>
+  <si>
+    <t>ନିଶିଣ୍ଟାକୋଇଲି-କଟିକଟା |</t>
+  </si>
+  <si>
+    <t>ନିଶ୍ଚିନ୍ତକୋଇଲି-ତରାଟ |</t>
+  </si>
+  <si>
+    <t>ଚନ୍ଦ୍ରଦେଇପୁର  (ସାଲେପୁର) -ମହଜନପୁର |</t>
+  </si>
+  <si>
+    <t>ଚନ୍ଦ୍ରଦେଇପୁର  (ସାଲେପୁର) -ନାଇଗୁଆନ୍ |</t>
+  </si>
+  <si>
+    <t>ଚନ୍ଦ୍ରଦେଇପୁର  (ସାଲେପୁର) -ସୁଧାଖଣ୍ଡା |</t>
+  </si>
+  <si>
+    <t>ଟାଙ୍ଗୀ ଚୌଦ୍ୱାର -କାକାଡି |</t>
+  </si>
+  <si>
+    <t>ଟାଙ୍ଗୀ ଚୌଦ୍ୱାର -ବାଦାସାମନ୍ତପୁର |</t>
+  </si>
+  <si>
+    <t>ଟାଙ୍ଗୀ ଚୌଦ୍ୱାର -କରଞ୍ଜୀ |</t>
+  </si>
+  <si>
+    <t>ଟାଙ୍ଗୀ ଚୌଦ୍ୱାର - ଜରିପଦା  |</t>
+  </si>
+  <si>
+    <t>ପଞ୍ଚାଗାନ୍ (ଟିଗିରିଆ) -ହାଣ୍ଡପସି |</t>
+  </si>
+  <si>
+    <t>ପଞ୍ଚାଗାନ୍ (ଟିଗିରିଆ) -ଜମାଦେଇପୁର  |</t>
+  </si>
+  <si>
+    <t>ପଞ୍ଚାଗାନ୍ (ଟିଗିରିଆ) - ଗଦାଧରପୁର  |</t>
+  </si>
+  <si>
+    <t>ଆଠଗଡ -କଟକ |</t>
+  </si>
+  <si>
+    <t>ବାଙ୍କୀ  -କଟକ |</t>
+  </si>
+  <si>
+    <t>ଦମପରା-କଟକ |</t>
+  </si>
+  <si>
+    <t>ମାହାଙ୍ଗା  -କଟକ |</t>
+  </si>
+  <si>
+    <t>ନିଆଳି  -କଟକ |</t>
+  </si>
+  <si>
+    <t>ନିଶ୍ଚିନ୍ତକୋଇଲି -କଟକ |</t>
+  </si>
+  <si>
+    <t>ଟାଙ୍ଗୀ ଚୌଦ୍ୱାର -କଟକ |</t>
+  </si>
+  <si>
+    <t>ଭାୟା - ବନାବିଧ୍ୟାଧରପୁର-ଗାତିରାଉଟପାଟନା-ମାତାଗାଜାପୁର-ପରମାନସା-ବିରିବତୀ-କନ୍ଦରପୁର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଡୋରାଡା-କୁଲାଇଲୋ-ଭୋଗ୍ରା ଏବଂ ପଛ ଡାଲାବାଗା-ଖୁଣ୍ଟୁନି-ରାଧାକିଶୋରପୁର-ଓରଣ୍ଡା-ଗୁରୁଦିଜାଟିଆ-ଛାଗୋନ୍-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ରାଧାଗୋବିନ୍ଦପୁର-ରାଜନାନଗର-ମହାକାଲାବାସ୍ତା-ଘଣ୍ଟିଖଲା-ଧୁରୁସିଆ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସାମସପୁର-ଇଚାପୁର-ଜେନାଡେଡେଶ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସୁନାପାଲା ଛକା-ଇଚାପୁର-ମଙ୍ଗରାଜପୁର-ଜାଜିଆ-କରାଡିବନ୍ଧା-ସାସଙ୍ଗା-ଭଟ୍ଟାରିକା-ଗେମି-କାନ୍ଦା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବ୍ରହ୍ମପୁରା-କିଆପାଲା-ବାରପୁଟ-ନୁଆଗାନ୍-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସୁବାମପୁର-ରତାଗର-ବୃନ୍ଦାବନ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଓଷ୍ଟିଆ-କାଦଲିବାଡି-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଆରିଲୋ-ଗାବାବାସ୍ତା-ଦେଓକାଲୀ-କୋରାକାନା-ସିଙ୍ଗହୋଲ-ବାଇଲୋ ବଜାର-ଉଲାର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ପଞ୍ଚୁପାଲ-ବେଲଗାଖିଆ-ଗୋବିନ୍ଦପୁର ଏବଂ ରତନଗର-ମୁଣ୍ଡାଲି-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଗୋବିନ୍ଦପୁର-ଦୁଲାନାପୁର-ତାଲାବସ୍ତା-ବିଲିପଡା-ହରିରାଜପୁର ଏବଂ ସିମିଲିପୁର-ଘସିପୁଟ-କୁସପାଙ୍ଗି-ଭାଗିପୁର-ବାମାରା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଘାସିପୁଟ-ନୁରସିଂହ-ଦୁର୍ଗାପୁର-ରାଗଡି-ଗୋପାଳପୁର-ଧନସାରା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବାଗଲପୁର-ବାଦପଟାସୁନ୍ଦର-har ାରପଡା-ଗୋବିନ୍ଦପୁର-ନୁଆଗାଙ୍ଗ୍ରାମ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବ୍ରାହ୍ମଣସାଲୋ-ବ୍ରାହ୍ମଣବତୀ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଉର୍ଧା-ଆଦାସପୁର-ଉତ୍ତରାଣା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କୁସୁପୁର-ବାଲିଚନ୍ଦ୍ରପୁର-ପାନସପୁର-ଲଲିତଗିରି-ଓଲାକାନା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ପାକାପଡା ପାଟନା, ନିଜିଗର-ବାଦାବୁଇନ୍, ରଣସିଗପୁର-ଜାଜିବନ୍ଧା-ବିରସିଂହପୁର-ଭୁସ୍କା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ନୁଆପାଟନା-ନିମାସାହି-କୋକଲବା-କଥଖୁଣ୍ଟା-ବାଲିସାହି-ସାରଦାପୁର-ଯୋଡମ୍-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବିଲାସୁନି-ରାନିଓଲା-କାସରଡା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଜଲାରପୁର-ମାଧବା-ରତନପୁର-କେ ପ୍ରସାଦ-ବିନିଶପୁର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଜଲାରପୁର-କାପାସୀ-ସାଧନା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା - ବାହରାନା- ପୋଖରିଗାଓଁ-ପହଙ୍ଗା-ଏକବେରୁଆନ୍-ସୀଥାଲୋ-ସାଗାଦାଇଲୋ-ବିଲାସୁନି-ଆଲାନା-ଆନ୍ଲୋ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ନେମାଲ-ସାନ୍ତାପୁର-ପାଲଡା-ବାବୁଜାଙ୍ଗ-ମଣିଜଙ୍ଗା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବୁହାଲୋ-ତିଲକାନା-ବାନ୍ଧକାଟିଆ-ତରାଟ-ଅସୁରଶ୍ୱର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବୁହାଲୋ-ନେମାଲୋ-ନାଗାସପୁର-ଦ ud ଦପୁର-ନରେନ୍ଦ୍ରପୁର-ଅର୍ଟି-କେନୋ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବୋଡାମୁଣ୍ଡେଇ- ପାଇକଲ୍-ରାଇସୁଙ୍ଗୁରା-ମିର୍ଜାପୁର-ଭୀମଦାସପୁର-ସିଦ୍ଧୋ-ଖାନିପୁର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ବାଲିସାହି-ସିସୁଆ-ଟାରିଟୋ-ରତିଲୋ-ପୁରୂନାହାଟ-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କୋଟାସାହି-କାନହିପୁର-ସାଲାଗାଓଁ-ନାଖ୍ରା-ଆଗ୍ରାହତ-ଇନ୍ଦ୍ରାନିପାଟନ-କାୟଲପଡା-ଧବାଲେଶ୍ୱର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କୋଟାସାହି-କାନହିପୁର- ଗରୁଡାଗାଓନ୍-ବରହମପୁର-ମହିସାଲାଣ୍ଡା-ଶଙ୍କରପୁର-ମଙ୍ଗରାଜପୁର-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କୋଟାସାହି-ଉଚାପଡା-ମାଗୁରା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କୋଟାସାହି-କାନହିପୁର-ଗାରୁଦାଗୋନ୍-ସଫା-</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ନୁଆସାଦକ୍-ଗୋଡିଜରିଆ-ଭିରୁଦା-ଆଚାଲକୋଟ୍-</t>
+  </si>
+  <si>
+    <t>ଭାୟା - ପୁସପାଙ୍ଗି-ଗୋଡିସାହି-ସାନ୍ଧପୁର-ତ୍ରିସୁଲିଆ |</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଖୁଣ୍ଟାକାଟା-ଅଟାଗର-କୁଲାଇଲୋ-ଖୁଣ୍ଟୁନି-ବାଲି-ଚୌଦ୍ୱାର-ମାଙ୍ଗୁଲି-ଜଗତପୁର |</t>
+  </si>
+  <si>
+    <t>ଭାୟା - କପିଲାଶ ରୋଡ-ସୋସିଆପଡା-ହରିପୁର-ସଫା-ବିସି ନାହକାନି-ହଳଦିବସନ୍ତ -କାମୋମଗୋ-ଡାଲିଜୋଡା-ବରହମପୁର-ଚାରବାଟିଆ-ଆଗ୍ରାହାଟ - ଏ ର ସି ଚୌଦ୍ୱାର- ମଙ୍ଗୁଳି -ଜଗତପୁର |</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସିସୁଆ-ଭଟ୍ଟପଡା-ଖରାହିଆ-ଭଇରପୁର -ଜଗତପୁର |</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କେନ୍ଦୁପଟାନା -ସାଲେପୁର-ସିସୁଆ-ଭଟ୍ଟପଡା-ଖରାହିଆ ଭଇରପୁର -ଜଗତପୁର</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଅଡସପୁର -ଓଲଟପୁର-କଣ୍ଟାପଡା-ସୁନ୍ଦରଗାଁ - ବ୍ରାହ୍ମଣଝରିଲୋ -ଫୁଲନଖରା-ଗୋପାଳପୁର</t>
+  </si>
+  <si>
+    <t>ଭାୟା-ରୁଖପଡା-ବାଗଧାରିଆ-ଚମ୍ପେଶ୍ୱର-ବାଲିଜାରୀ-ବଡମ୍ବା-ମଣିବନ୍ଧା-ନୁଆପାଟନା-ତିଗିରା- ଖୁଣ୍ଟକଟା -ଆଠଗଡ-କୁଲେଇଲ -ଖୁଣ୍ଟୁଣି-ବାଲି- ଚୌଦ୍ୱାର-ମଙ୍ଗୁଲି-ଜଗତପୁର</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଧର୍ମଘଟପୁର-ମନୋହରପୁର-ସାଲେପୁର -ସିସୁଆ-ଭାଟପଡା -ଖରଡିଆ  - ଭଇରପୁର -ଜଗତପୁର</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ସୁନ୍ଦରଗାଓଁ-ବ୍ରାହ୍ମଣଜ୍ରିଲୋ-ଫୁଲନଖରା- ଗୋପାଳପୁର |</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଜଟାମୁଣ୍ଡିଆ-ପଥପୁର -ଦେବିଦ୍ୱାର-ବଅଁରା- ଗୋବିନ୍ଦପୁର-ଗୋଡିସାହି-ସନ୍ଧପୁର-ତ୍ରିସୁଳିଆ |</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଧୋବନିନାଲା-ମାନୀଆବନ୍ଧ-ବିଧରପୁର-ନୂଆପାଟଣା -ବିରିପୁଟ-ନୂଆସଡ଼କ 
+ -ଖୁଣ୍ଟାକାଟା-ଆଠଗଡ-କାଣ୍ଟୋଲ-କାରିକୋଲ-ମହାକାଲାବାସ୍ତା-ନିଧିପୁର -କାଖଡି</t>
+  </si>
+  <si>
+    <t>ଭାୟା- କାଣ୍ଟୋଲ-କାଖଡି-ମହାକାଲାବାସ୍ତା |</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ନିଜିଗଡ଼-ପୁରାଣତିଗିରିଆ-ପାଇକାନାରା-ବାଦାନୁଆପୁଟ-ସନ୍ଥିପାଲା-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1061,6 +1432,12 @@
       <sz val="12"/>
       <name val="Arial MT"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1095,7 +1472,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1237,9 +1614,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1250,6 +1624,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1316,7 +1693,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1351,7 +1728,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1528,34 +1905,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView zoomScale="77" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="23.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.54296875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.453125" customWidth="1"/>
-    <col min="8" max="8" width="19.54296875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.649999999999999" customHeight="1">
+    <row r="1" spans="1:9" ht="18.600000000000001" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2651,77 +3028,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0948853-C366-475C-B33B-E7FBE20B0E7F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="M38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="0" style="11" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="11"/>
-    <col min="4" max="4" width="13.6328125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" style="11" customWidth="1"/>
-    <col min="7" max="7" width="19.7265625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1796875" style="11" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16.81640625" style="11" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" style="11"/>
+    <col min="4" max="4" width="13.6640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" style="11" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" style="11" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="40" style="11" customWidth="1"/>
     <col min="13" max="13" width="34" style="11" customWidth="1"/>
-    <col min="14" max="14" width="78.08984375" style="11" customWidth="1"/>
-    <col min="15" max="15" width="68.26953125" style="11" customWidth="1"/>
-    <col min="16" max="16" width="18.81640625" style="11" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="16.54296875" style="11" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.7265625" style="11"/>
+    <col min="14" max="14" width="78.109375" style="11" customWidth="1"/>
+    <col min="15" max="15" width="68.21875" style="11" customWidth="1"/>
+    <col min="16" max="16" width="18.77734375" style="11" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5546875" style="11" hidden="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.77734375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="23">
-      <c r="A1" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-    </row>
-    <row r="2" spans="1:17" ht="23">
-      <c r="A2" s="25" t="s">
+    <row r="1" spans="1:17" ht="22.8">
+      <c r="A1" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+    </row>
+    <row r="2" spans="1:17" ht="22.8">
+      <c r="A2" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-    </row>
-    <row r="3" spans="1:17" ht="31">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+    </row>
+    <row r="3" spans="1:17" ht="31.2">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -2774,7 +3151,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="31">
+    <row r="4" spans="1:17" ht="30">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -2808,15 +3185,19 @@
       <c r="L4" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="M4" s="10"/>
+      <c r="M4" s="10" t="s">
+        <v>360</v>
+      </c>
       <c r="N4" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="O4" s="15"/>
+      <c r="O4" s="15" t="s">
+        <v>392</v>
+      </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="17"/>
     </row>
-    <row r="5" spans="1:17" ht="77.5">
+    <row r="5" spans="1:17" ht="105">
       <c r="A5" s="10">
         <v>2</v>
       </c>
@@ -2850,17 +3231,21 @@
       <c r="L5" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="10" t="s">
+        <v>348</v>
+      </c>
       <c r="N5" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="O5" s="15"/>
+      <c r="O5" s="15" t="s">
+        <v>335</v>
+      </c>
       <c r="P5" s="18" t="s">
         <v>169</v>
       </c>
       <c r="Q5" s="10"/>
     </row>
-    <row r="6" spans="1:17" ht="46.5">
+    <row r="6" spans="1:17" ht="45">
       <c r="A6" s="10">
         <v>3</v>
       </c>
@@ -2887,22 +3272,26 @@
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
-      <c r="K6" s="24" t="str">
+      <c r="K6" s="10" t="str">
         <f t="shared" si="0"/>
         <v>CT003</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="M6" s="10"/>
+      <c r="M6" s="10" t="s">
+        <v>361</v>
+      </c>
       <c r="N6" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="O6" s="15"/>
+      <c r="O6" s="15" t="s">
+        <v>336</v>
+      </c>
       <c r="P6" s="16"/>
       <c r="Q6" s="10"/>
     </row>
-    <row r="7" spans="1:17" ht="31">
+    <row r="7" spans="1:17" ht="30">
       <c r="A7" s="10">
         <v>4</v>
       </c>
@@ -2929,22 +3318,26 @@
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="24" t="str">
+      <c r="K7" s="10" t="str">
         <f t="shared" si="0"/>
         <v>CT004</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="M7" s="15"/>
+      <c r="M7" s="10" t="s">
+        <v>362</v>
+      </c>
       <c r="N7" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="O7" s="15"/>
+      <c r="O7" s="15" t="s">
+        <v>337</v>
+      </c>
       <c r="P7" s="16"/>
       <c r="Q7" s="10"/>
     </row>
-    <row r="8" spans="1:17" ht="31">
+    <row r="8" spans="1:17" ht="30">
       <c r="A8" s="10">
         <v>5</v>
       </c>
@@ -2971,18 +3364,22 @@
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="24" t="str">
+      <c r="K8" s="10" t="str">
         <f t="shared" si="0"/>
         <v>CT005</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="M8" s="15"/>
+      <c r="M8" s="10" t="s">
+        <v>350</v>
+      </c>
       <c r="N8" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="O8" s="15"/>
+      <c r="O8" s="15" t="s">
+        <v>393</v>
+      </c>
       <c r="P8" s="16"/>
       <c r="Q8" s="10"/>
     </row>
@@ -3013,18 +3410,22 @@
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="24" t="str">
+      <c r="K9" s="10" t="str">
         <f t="shared" si="0"/>
         <v>CT006</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="M9" s="15"/>
+      <c r="M9" s="10" t="s">
+        <v>349</v>
+      </c>
       <c r="N9" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="O9" s="15"/>
+      <c r="O9" s="15" t="s">
+        <v>394</v>
+      </c>
       <c r="P9" s="16"/>
       <c r="Q9" s="10"/>
     </row>
@@ -3062,15 +3463,19 @@
       <c r="L10" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="M10" s="15"/>
+      <c r="M10" s="28" t="s">
+        <v>363</v>
+      </c>
       <c r="N10" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="O10" s="15"/>
+      <c r="O10" s="15" t="s">
+        <v>395</v>
+      </c>
       <c r="P10" s="16"/>
       <c r="Q10" s="10"/>
     </row>
-    <row r="11" spans="1:17" ht="62">
+    <row r="11" spans="1:17" ht="60">
       <c r="A11" s="10">
         <v>5</v>
       </c>
@@ -3097,22 +3502,26 @@
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="24" t="str">
+      <c r="K11" s="10" t="str">
         <f t="shared" si="0"/>
         <v>CT008</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="M11" s="15"/>
+      <c r="M11" s="28" t="s">
+        <v>351</v>
+      </c>
       <c r="N11" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="O11" s="15"/>
+      <c r="O11" s="15" t="s">
+        <v>352</v>
+      </c>
       <c r="P11" s="19"/>
       <c r="Q11" s="10"/>
     </row>
-    <row r="12" spans="1:17" ht="31">
+    <row r="12" spans="1:17" ht="30">
       <c r="A12" s="10">
         <v>6</v>
       </c>
@@ -3146,15 +3555,19 @@
       <c r="L12" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="M12" s="15"/>
+      <c r="M12" s="10" t="s">
+        <v>353</v>
+      </c>
       <c r="N12" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="O12" s="15"/>
+      <c r="O12" s="15" t="s">
+        <v>338</v>
+      </c>
       <c r="P12" s="19"/>
       <c r="Q12" s="10"/>
     </row>
-    <row r="13" spans="1:17" ht="31">
+    <row r="13" spans="1:17" ht="30">
       <c r="A13" s="10">
         <v>10</v>
       </c>
@@ -3181,22 +3594,26 @@
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="24" t="str">
+      <c r="K13" s="10" t="str">
         <f t="shared" si="0"/>
         <v>CT010</v>
       </c>
       <c r="L13" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="M13" s="15"/>
+      <c r="M13" s="10" t="s">
+        <v>354</v>
+      </c>
       <c r="N13" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="O13" s="15"/>
+      <c r="O13" s="15" t="s">
+        <v>339</v>
+      </c>
       <c r="P13" s="19"/>
       <c r="Q13" s="10"/>
     </row>
-    <row r="14" spans="1:17" ht="31">
+    <row r="14" spans="1:17" ht="30">
       <c r="A14" s="10">
         <v>7</v>
       </c>
@@ -3230,15 +3647,19 @@
       <c r="L14" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="M14" s="15"/>
+      <c r="M14" s="10" t="s">
+        <v>355</v>
+      </c>
       <c r="N14" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="O14" s="15"/>
+      <c r="O14" s="15" t="s">
+        <v>396</v>
+      </c>
       <c r="P14" s="19"/>
       <c r="Q14" s="10"/>
     </row>
-    <row r="15" spans="1:17" ht="31">
+    <row r="15" spans="1:17" ht="45">
       <c r="A15" s="10">
         <v>8</v>
       </c>
@@ -3265,18 +3686,22 @@
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="24" t="str">
+      <c r="K15" s="10" t="str">
         <f t="shared" si="0"/>
         <v>CT012</v>
       </c>
       <c r="L15" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="M15" s="15"/>
+      <c r="M15" s="10" t="s">
+        <v>364</v>
+      </c>
       <c r="N15" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="O15" s="20"/>
+      <c r="O15" s="20" t="s">
+        <v>340</v>
+      </c>
       <c r="P15" s="19"/>
       <c r="Q15" s="10"/>
     </row>
@@ -3314,11 +3739,15 @@
       <c r="L16" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="M16" s="15"/>
+      <c r="M16" s="10" t="s">
+        <v>319</v>
+      </c>
       <c r="N16" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="O16" s="15"/>
+      <c r="O16" s="15" t="s">
+        <v>397</v>
+      </c>
       <c r="P16" s="19"/>
       <c r="Q16" s="10"/>
     </row>
@@ -3356,11 +3785,15 @@
       <c r="L17" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="M17" s="15"/>
+      <c r="M17" s="10" t="s">
+        <v>320</v>
+      </c>
       <c r="N17" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="O17" s="15"/>
+      <c r="O17" s="15" t="s">
+        <v>398</v>
+      </c>
       <c r="P17" s="19"/>
       <c r="Q17" s="10"/>
     </row>
@@ -3391,22 +3824,26 @@
       </c>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
-      <c r="K18" s="24" t="str">
+      <c r="K18" s="10" t="str">
         <f t="shared" si="0"/>
         <v>CT015</v>
       </c>
       <c r="L18" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="M18" s="15"/>
+      <c r="M18" s="10" t="s">
+        <v>365</v>
+      </c>
       <c r="N18" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="O18" s="15"/>
+      <c r="O18" s="15" t="s">
+        <v>399</v>
+      </c>
       <c r="P18" s="19"/>
       <c r="Q18" s="10"/>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" ht="30">
       <c r="A19" s="10">
         <v>16</v>
       </c>
@@ -3433,18 +3870,22 @@
       </c>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
-      <c r="K19" s="24" t="str">
+      <c r="K19" s="10" t="str">
         <f t="shared" si="0"/>
         <v>CT016</v>
       </c>
       <c r="L19" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="M19" s="15"/>
+      <c r="M19" s="10" t="s">
+        <v>321</v>
+      </c>
       <c r="N19" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="O19" s="15"/>
+      <c r="O19" s="15" t="s">
+        <v>400</v>
+      </c>
       <c r="P19" s="19"/>
       <c r="Q19" s="10"/>
     </row>
@@ -3475,18 +3916,22 @@
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
-      <c r="K20" s="24" t="str">
+      <c r="K20" s="10" t="str">
         <f t="shared" si="0"/>
         <v>CT017</v>
       </c>
       <c r="L20" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="M20" s="15"/>
+      <c r="M20" s="10" t="s">
+        <v>357</v>
+      </c>
       <c r="N20" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="O20" s="15"/>
+      <c r="O20" s="15" t="s">
+        <v>341</v>
+      </c>
       <c r="P20" s="19"/>
       <c r="Q20" s="10"/>
     </row>
@@ -3524,15 +3969,19 @@
       <c r="L21" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="M21" s="15"/>
+      <c r="M21" s="10" t="s">
+        <v>322</v>
+      </c>
       <c r="N21" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="O21" s="15"/>
+      <c r="O21" s="15" t="s">
+        <v>401</v>
+      </c>
       <c r="P21" s="19"/>
       <c r="Q21" s="10"/>
     </row>
-    <row r="22" spans="1:17" ht="31">
+    <row r="22" spans="1:17" ht="30">
       <c r="A22" s="10">
         <v>12</v>
       </c>
@@ -3559,18 +4008,22 @@
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
-      <c r="K22" s="24" t="str">
+      <c r="K22" s="10" t="str">
         <f t="shared" si="0"/>
         <v>CT019</v>
       </c>
       <c r="L22" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="M22" s="15"/>
+      <c r="M22" s="10" t="s">
+        <v>358</v>
+      </c>
       <c r="N22" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="O22" s="15"/>
+      <c r="O22" s="15" t="s">
+        <v>402</v>
+      </c>
       <c r="P22" s="19"/>
       <c r="Q22" s="10"/>
     </row>
@@ -3601,18 +4054,22 @@
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
-      <c r="K23" s="24" t="str">
+      <c r="K23" s="10" t="str">
         <f t="shared" si="0"/>
         <v>CT020</v>
       </c>
       <c r="L23" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="M23" s="15"/>
+      <c r="M23" s="10" t="s">
+        <v>359</v>
+      </c>
       <c r="N23" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="O23" s="15"/>
+      <c r="O23" s="15" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="10"/>
@@ -3639,18 +4096,22 @@
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
-      <c r="K24" s="24" t="str">
+      <c r="K24" s="10" t="str">
         <f t="shared" ref="K24:K30" si="1">E24&amp;H24</f>
         <v>CT021</v>
       </c>
       <c r="L24" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="M24" s="15"/>
+      <c r="M24" s="10" t="s">
+        <v>323</v>
+      </c>
       <c r="N24" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="O24" s="15"/>
+      <c r="O24" s="15" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="10"/>
@@ -3684,11 +4145,15 @@
       <c r="L25" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="M25" s="15"/>
+      <c r="M25" s="10" t="s">
+        <v>324</v>
+      </c>
       <c r="N25" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="O25" s="15"/>
+      <c r="O25" s="15" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="10"/>
@@ -3715,20 +4180,24 @@
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
-      <c r="K26" s="24" t="str">
+      <c r="K26" s="10" t="str">
         <f t="shared" si="1"/>
         <v>CT023</v>
       </c>
       <c r="L26" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="M26" s="15"/>
+      <c r="M26" s="10" t="s">
+        <v>325</v>
+      </c>
       <c r="N26" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="O26" s="15"/>
-    </row>
-    <row r="27" spans="1:17" ht="31">
+      <c r="O26" s="15" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="30">
       <c r="A27" s="10"/>
       <c r="B27" s="10">
         <v>24</v>
@@ -3753,18 +4222,22 @@
       </c>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="24" t="str">
+      <c r="K27" s="10" t="str">
         <f t="shared" si="1"/>
         <v>CT024</v>
       </c>
       <c r="L27" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="M27" s="15"/>
+      <c r="M27" s="10" t="s">
+        <v>366</v>
+      </c>
       <c r="N27" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="O27" s="15"/>
+      <c r="O27" s="15" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="10"/>
@@ -3798,13 +4271,17 @@
       <c r="L28" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="M28" s="15"/>
+      <c r="M28" s="10" t="s">
+        <v>367</v>
+      </c>
       <c r="N28" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="O28" s="15"/>
-    </row>
-    <row r="29" spans="1:17" ht="31">
+      <c r="O28" s="15" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="30">
       <c r="A29" s="10"/>
       <c r="B29" s="10">
         <v>26</v>
@@ -3829,18 +4306,22 @@
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
-      <c r="K29" s="24" t="str">
+      <c r="K29" s="10" t="str">
         <f t="shared" si="1"/>
         <v>CT026</v>
       </c>
       <c r="L29" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="M29" s="15"/>
+      <c r="M29" s="10" t="s">
+        <v>368</v>
+      </c>
       <c r="N29" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="O29" s="15"/>
+      <c r="O29" s="15" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="10"/>
@@ -3874,13 +4355,17 @@
       <c r="L30" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="M30" s="15"/>
+      <c r="M30" s="10" t="s">
+        <v>326</v>
+      </c>
       <c r="N30" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="O30" s="15"/>
-    </row>
-    <row r="31" spans="1:17" ht="31">
+      <c r="O30" s="15" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="30">
       <c r="A31" s="10"/>
       <c r="B31" s="10">
         <v>28</v>
@@ -3905,20 +4390,24 @@
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
-      <c r="K31" s="24" t="str">
+      <c r="K31" s="10" t="str">
         <f t="shared" ref="K31:K32" si="2">E31&amp;H31</f>
         <v>CT028</v>
       </c>
       <c r="L31" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="M31" s="15"/>
+      <c r="M31" s="10" t="s">
+        <v>369</v>
+      </c>
       <c r="N31" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="O31" s="15"/>
-    </row>
-    <row r="32" spans="1:17">
+      <c r="O31" s="15" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="30">
       <c r="A32" s="10"/>
       <c r="B32" s="10">
         <v>29</v>
@@ -3943,18 +4432,22 @@
       </c>
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
-      <c r="K32" s="24" t="str">
+      <c r="K32" s="10" t="str">
         <f t="shared" si="2"/>
         <v>CT029</v>
       </c>
       <c r="L32" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="M32" s="15"/>
+      <c r="M32" s="10" t="s">
+        <v>327</v>
+      </c>
       <c r="N32" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="O32" s="15"/>
+      <c r="O32" s="15" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="10"/>
@@ -3988,11 +4481,15 @@
       <c r="L33" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="M33" s="22"/>
+      <c r="M33" s="22" t="s">
+        <v>328</v>
+      </c>
       <c r="N33" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="O33" s="15"/>
+      <c r="O33" s="15" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="10"/>
@@ -4019,18 +4516,22 @@
       </c>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
-      <c r="K34" s="24" t="str">
+      <c r="K34" s="10" t="str">
         <f t="shared" si="3"/>
         <v>CT031</v>
       </c>
       <c r="L34" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="M34" s="22"/>
+      <c r="M34" s="22" t="s">
+        <v>329</v>
+      </c>
       <c r="N34" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="O34" s="15"/>
+      <c r="O34" s="15" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="10"/>
@@ -4064,13 +4565,17 @@
       <c r="L35" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="M35" s="22"/>
+      <c r="M35" s="22" t="s">
+        <v>370</v>
+      </c>
       <c r="N35" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="O35" s="15"/>
-    </row>
-    <row r="36" spans="1:15" ht="31">
+      <c r="O35" s="15" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="30">
       <c r="A36" s="10"/>
       <c r="B36" s="10">
         <v>33</v>
@@ -4095,18 +4600,22 @@
       </c>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
-      <c r="K36" s="24" t="str">
+      <c r="K36" s="10" t="str">
         <f t="shared" si="3"/>
         <v>CT033</v>
       </c>
       <c r="L36" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="M36" s="22"/>
+      <c r="M36" s="22" t="s">
+        <v>371</v>
+      </c>
       <c r="N36" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="O36" s="15"/>
+      <c r="O36" s="15" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="10"/>
@@ -4133,18 +4642,22 @@
       </c>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
-      <c r="K37" s="24" t="str">
+      <c r="K37" s="10" t="str">
         <f t="shared" si="3"/>
         <v>CT034</v>
       </c>
       <c r="L37" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="M37" s="22"/>
+      <c r="M37" s="22" t="s">
+        <v>372</v>
+      </c>
       <c r="N37" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="O37" s="15"/>
+      <c r="O37" s="15" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="10"/>
@@ -4178,13 +4691,17 @@
       <c r="L38" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="M38" s="22"/>
+      <c r="M38" s="22" t="s">
+        <v>373</v>
+      </c>
       <c r="N38" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="O38" s="15"/>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="O38" s="15" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="30">
       <c r="A39" s="10"/>
       <c r="B39" s="10">
         <v>36</v>
@@ -4209,20 +4726,24 @@
       </c>
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
-      <c r="K39" s="24" t="str">
+      <c r="K39" s="10" t="str">
         <f t="shared" si="3"/>
         <v>CT036</v>
       </c>
       <c r="L39" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="M39" s="22"/>
+      <c r="M39" s="22" t="s">
+        <v>374</v>
+      </c>
       <c r="N39" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="O39" s="15"/>
-    </row>
-    <row r="40" spans="1:15" ht="31">
+      <c r="O39" s="15" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="30">
       <c r="A40" s="10"/>
       <c r="B40" s="10">
         <v>37</v>
@@ -4247,20 +4768,24 @@
       </c>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
-      <c r="K40" s="24" t="str">
+      <c r="K40" s="10" t="str">
         <f t="shared" si="3"/>
         <v>CT037</v>
       </c>
       <c r="L40" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="M40" s="10"/>
+      <c r="M40" s="10" t="s">
+        <v>375</v>
+      </c>
       <c r="N40" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="O40" s="15"/>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="O40" s="15" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="30">
       <c r="A41" s="10"/>
       <c r="B41" s="10">
         <v>38</v>
@@ -4292,13 +4817,17 @@
       <c r="L41" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="M41" s="10"/>
+      <c r="M41" s="10" t="s">
+        <v>376</v>
+      </c>
       <c r="N41" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="O41" s="15"/>
-    </row>
-    <row r="42" spans="1:15" ht="31">
+      <c r="O41" s="15" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15" customHeight="1">
       <c r="A42" s="10"/>
       <c r="B42" s="10">
         <v>39</v>
@@ -4323,20 +4852,24 @@
       </c>
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
-      <c r="K42" s="24" t="str">
+      <c r="K42" s="10" t="str">
         <f t="shared" si="3"/>
         <v>CT039</v>
       </c>
       <c r="L42" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="M42" s="10"/>
+      <c r="M42" s="10" t="s">
+        <v>377</v>
+      </c>
       <c r="N42" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="O42" s="15"/>
-    </row>
-    <row r="43" spans="1:15" ht="31">
+      <c r="O42" s="15" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="30">
       <c r="A43" s="10"/>
       <c r="B43" s="10">
         <v>40</v>
@@ -4361,20 +4894,24 @@
       </c>
       <c r="I43" s="10"/>
       <c r="J43" s="10"/>
-      <c r="K43" s="24" t="str">
+      <c r="K43" s="10" t="str">
         <f t="shared" ref="K43:K50" si="4">E43&amp;H43</f>
         <v>CT040</v>
       </c>
       <c r="L43" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="M43" s="10"/>
+      <c r="M43" s="10" t="s">
+        <v>378</v>
+      </c>
       <c r="N43" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="O43" s="15"/>
-    </row>
-    <row r="44" spans="1:15" ht="31">
+      <c r="O43" s="15" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="30">
       <c r="A44" s="10"/>
       <c r="B44" s="10">
         <v>41</v>
@@ -4406,11 +4943,15 @@
       <c r="L44" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="M44" s="10"/>
+      <c r="M44" s="10" t="s">
+        <v>379</v>
+      </c>
       <c r="N44" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="O44" s="15"/>
+      <c r="O44" s="15" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="45" spans="1:15">
       <c r="A45" s="10"/>
@@ -4444,11 +4985,15 @@
       <c r="L45" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="M45" s="10"/>
+      <c r="M45" s="10" t="s">
+        <v>381</v>
+      </c>
       <c r="N45" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="O45" s="15"/>
+      <c r="O45" s="15" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="46" spans="1:15">
       <c r="A46" s="10"/>
@@ -4475,18 +5020,22 @@
       </c>
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
-      <c r="K46" s="24" t="str">
+      <c r="K46" s="10" t="str">
         <f t="shared" si="4"/>
         <v>CT043</v>
       </c>
       <c r="L46" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="M46" s="10"/>
+      <c r="M46" s="10" t="s">
+        <v>380</v>
+      </c>
       <c r="N46" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="O46" s="15"/>
+      <c r="O46" s="15" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="47" spans="1:15">
       <c r="A47" s="10"/>
@@ -4520,11 +5069,15 @@
       <c r="L47" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="M47" s="10"/>
+      <c r="M47" s="10" t="s">
+        <v>330</v>
+      </c>
       <c r="N47" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="O47" s="15"/>
+      <c r="O47" s="15" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="48" spans="1:15">
       <c r="A48" s="10"/>
@@ -4551,20 +5104,24 @@
       </c>
       <c r="I48" s="10"/>
       <c r="J48" s="10"/>
-      <c r="K48" s="24" t="str">
+      <c r="K48" s="10" t="str">
         <f t="shared" si="4"/>
         <v>CT045</v>
       </c>
       <c r="L48" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="M48" s="10"/>
+      <c r="M48" s="10" t="s">
+        <v>382</v>
+      </c>
       <c r="N48" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="O48" s="15"/>
-    </row>
-    <row r="49" spans="1:15" ht="31">
+      <c r="O48" s="15" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="15" customHeight="1">
       <c r="A49" s="10"/>
       <c r="B49" s="10">
         <v>46</v>
@@ -4589,18 +5146,22 @@
       </c>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
-      <c r="K49" s="24" t="str">
+      <c r="K49" s="10" t="str">
         <f t="shared" si="4"/>
         <v>CT046</v>
       </c>
       <c r="L49" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="M49" s="10"/>
+      <c r="M49" s="10" t="s">
+        <v>383</v>
+      </c>
       <c r="N49" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="O49" s="15"/>
+      <c r="O49" s="15" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="50" spans="1:15">
       <c r="A50" s="10"/>
@@ -4634,28 +5195,32 @@
       <c r="L50" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="M50" s="10"/>
+      <c r="M50" s="10" t="s">
+        <v>384</v>
+      </c>
       <c r="N50" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="O50" s="15"/>
+      <c r="O50" s="15" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="51" spans="1:15">
-      <c r="A51" s="26"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="27"/>
-      <c r="J51" s="27"/>
-      <c r="K51" s="26"/>
-      <c r="L51" s="26"/>
-      <c r="M51" s="26"/>
-      <c r="N51" s="26"/>
-      <c r="O51" s="28"/>
+      <c r="A51" s="25"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="25"/>
+      <c r="M51" s="25"/>
+      <c r="N51" s="25"/>
+      <c r="O51" s="27"/>
     </row>
     <row r="52" spans="1:15">
       <c r="A52" s="10">
@@ -4692,13 +5257,17 @@
         <f>G52&amp;"-"&amp;D$14</f>
         <v>Athagarh-Cuttack</v>
       </c>
-      <c r="M52" s="15"/>
+      <c r="M52" s="15" t="s">
+        <v>385</v>
+      </c>
       <c r="N52" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="O52" s="15"/>
-    </row>
-    <row r="53" spans="1:15" ht="31">
+      <c r="O52" s="15" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="30">
       <c r="A53" s="10">
         <v>31</v>
       </c>
@@ -4733,13 +5302,17 @@
         <f t="shared" ref="L53:L57" si="5">G53&amp;"-"&amp;D$14</f>
         <v>Badamba-Cuttack</v>
       </c>
-      <c r="M53" s="15"/>
+      <c r="M53" s="15" t="s">
+        <v>356</v>
+      </c>
       <c r="N53" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="O53" s="15"/>
-    </row>
-    <row r="54" spans="1:15" ht="31">
+      <c r="O53" s="15" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="30">
       <c r="A54" s="10">
         <v>32</v>
       </c>
@@ -4774,11 +5347,15 @@
         <f t="shared" si="5"/>
         <v>Banki-Cuttack</v>
       </c>
-      <c r="M54" s="15"/>
+      <c r="M54" s="15" t="s">
+        <v>386</v>
+      </c>
       <c r="N54" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="O54" s="15"/>
+      <c r="O54" s="15" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="55" spans="1:15">
       <c r="B55" s="10">
@@ -4812,11 +5389,15 @@
         <f t="shared" si="5"/>
         <v>Dampara-Cuttack</v>
       </c>
-      <c r="M55" s="15"/>
+      <c r="M55" s="15" t="s">
+        <v>387</v>
+      </c>
       <c r="N55" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="O55" s="15"/>
+      <c r="O55" s="15" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="56" spans="1:15">
       <c r="B56" s="10">
@@ -4850,13 +5431,17 @@
         <f t="shared" si="5"/>
         <v>Kantapada-Cuttack</v>
       </c>
-      <c r="M56" s="15"/>
+      <c r="M56" s="15" t="s">
+        <v>331</v>
+      </c>
       <c r="N56" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="O56" s="15"/>
-    </row>
-    <row r="57" spans="1:15" ht="31">
+      <c r="O56" s="15" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="30">
       <c r="B57" s="10">
         <v>53</v>
       </c>
@@ -4888,13 +5473,17 @@
         <f t="shared" si="5"/>
         <v>Mahanga-Cuttack</v>
       </c>
-      <c r="M57" s="15"/>
+      <c r="M57" s="15" t="s">
+        <v>388</v>
+      </c>
       <c r="N57" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="O57" s="15"/>
-    </row>
-    <row r="58" spans="1:15" ht="46.5">
+      <c r="O57" s="15" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="45">
       <c r="B58" s="10">
         <v>54</v>
       </c>
@@ -4926,13 +5515,17 @@
         <f t="shared" ref="L58:L63" si="7">G58&amp;"-"&amp;D$14</f>
         <v>Narsinghpur-Cuttack</v>
       </c>
-      <c r="M58" s="15"/>
+      <c r="M58" s="15" t="s">
+        <v>332</v>
+      </c>
       <c r="N58" s="23" t="s">
         <v>302</v>
       </c>
-      <c r="O58" s="15"/>
-    </row>
-    <row r="59" spans="1:15" ht="31">
+      <c r="O58" s="15" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="30">
       <c r="B59" s="10">
         <v>55</v>
       </c>
@@ -4964,11 +5557,15 @@
         <f t="shared" si="7"/>
         <v>Niali-Cuttack</v>
       </c>
-      <c r="M59" s="15"/>
+      <c r="M59" s="15" t="s">
+        <v>389</v>
+      </c>
       <c r="N59" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="O59" s="15"/>
+      <c r="O59" s="15" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="60" spans="1:15">
       <c r="B60" s="10">
@@ -5002,11 +5599,15 @@
         <f t="shared" si="7"/>
         <v>Nischintakoili-Cuttack</v>
       </c>
-      <c r="M60" s="15"/>
+      <c r="M60" s="15" t="s">
+        <v>390</v>
+      </c>
       <c r="N60" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="O60" s="15"/>
+      <c r="O60" s="15" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="61" spans="1:15">
       <c r="B61" s="10">
@@ -5040,13 +5641,17 @@
         <f t="shared" si="7"/>
         <v>Salepur-Cuttack</v>
       </c>
-      <c r="M61" s="15"/>
+      <c r="M61" s="15" t="s">
+        <v>333</v>
+      </c>
       <c r="N61" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="O61" s="15"/>
-    </row>
-    <row r="62" spans="1:15" ht="46.5">
+      <c r="O61" s="15" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="45">
       <c r="B62" s="10">
         <v>58</v>
       </c>
@@ -5078,13 +5683,17 @@
         <f t="shared" si="7"/>
         <v>Tangi-Chowdwar-Cuttack</v>
       </c>
-      <c r="M62" s="15"/>
+      <c r="M62" s="15" t="s">
+        <v>391</v>
+      </c>
       <c r="N62" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="O62" s="15"/>
-    </row>
-    <row r="63" spans="1:15">
+      <c r="O62" s="15" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="15" customHeight="1">
       <c r="B63" s="10">
         <v>59</v>
       </c>
@@ -5116,14 +5725,18 @@
         <f t="shared" si="7"/>
         <v>Tigiria-Cuttack</v>
       </c>
-      <c r="M63" s="15"/>
+      <c r="M63" s="15" t="s">
+        <v>334</v>
+      </c>
       <c r="N63" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="O63" s="10"/>
+      <c r="O63" s="10" t="s">
+        <v>425</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:R50" xr:uid="{C0948853-C366-475C-B33B-E7FBE20B0E7F}"/>
+  <autoFilter ref="A3:R50"/>
   <mergeCells count="3">
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A1:O1"/>

</xml_diff>